<commit_message>
Renamed "template file" instances to "experiment definition" as a result of feedback. Changed column headers to match ICE export / EDD bulk line creation script. Fixed a parse error encountered as a result of column header changes.
</commit_message>
<xml_diff>
--- a/main/fixtures/simple_template_file.xlsx
+++ b/main/fixtures/simple_template_file.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="51440" yWindow="4680" windowWidth="22480" windowHeight="7360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="simple_template_file.csv" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <t>Description blah blah</t>
   </si>
   <si>
-    <t>Strains</t>
+    <t>Part ID</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>